<commit_message>
added suymbols, segregated the html file, master dict(to work on)
</commit_message>
<xml_diff>
--- a/All.xlsx
+++ b/All.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Newfolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\screener\custom_screener_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AF6A6C-6E99-4814-9590-41C07FF1B02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB43EB16-07D7-4076-AD20-A77EF84113E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="4185" windowWidth="11670" windowHeight="11295" xr2:uid="{0348B957-CF79-4279-B861-6B8A209552E7}"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="28965" windowHeight="8055" xr2:uid="{0348B957-CF79-4279-B861-6B8A209552E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Stocks</t>
   </si>
@@ -48,6 +48,30 @@
   </si>
   <si>
     <t>RELIANCE.NS</t>
+  </si>
+  <si>
+    <t>JINDALSTEL</t>
+  </si>
+  <si>
+    <t>LICHSGFIN</t>
+  </si>
+  <si>
+    <t>ABB</t>
+  </si>
+  <si>
+    <t>UNITDSPR</t>
+  </si>
+  <si>
+    <t>RAMCOCEM</t>
+  </si>
+  <si>
+    <t>LTTS</t>
+  </si>
+  <si>
+    <t>BANKBARODA</t>
+  </si>
+  <si>
+    <t>COROMANDEL</t>
   </si>
 </sst>
 </file>
@@ -419,13 +443,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904BEEC-D85C-4382-B015-B596E311D931}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -443,6 +470,46 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed nifty indices as history was not available for past year, delete master at EOD
</commit_message>
<xml_diff>
--- a/All.xlsx
+++ b/All.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\screener\custom_screener_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\screener\orig\custom_screener_dhaval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB43EB16-07D7-4076-AD20-A77EF84113E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054596AB-E456-41DD-A234-DE742E16DF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3120" windowWidth="28965" windowHeight="8055" xr2:uid="{0348B957-CF79-4279-B861-6B8A209552E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0348B957-CF79-4279-B861-6B8A209552E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,20 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Stocks</t>
   </si>
   <si>
-    <t>Ticker</t>
-  </si>
-  <si>
     <t>RELIANCE</t>
   </si>
   <si>
-    <t>RELIANCE.NS</t>
-  </si>
-  <si>
     <t>JINDALSTEL</t>
   </si>
   <si>
@@ -72,6 +66,534 @@
   </si>
   <si>
     <t>COROMANDEL</t>
+  </si>
+  <si>
+    <t>GUJGASLTD</t>
+  </si>
+  <si>
+    <t>OBEROIRLTY</t>
+  </si>
+  <si>
+    <t>TITAN</t>
+  </si>
+  <si>
+    <t>NMDC</t>
+  </si>
+  <si>
+    <t>PEL</t>
+  </si>
+  <si>
+    <t>SBILIFE</t>
+  </si>
+  <si>
+    <t>AARTIIND</t>
+  </si>
+  <si>
+    <t>BAJAJFINSV</t>
+  </si>
+  <si>
+    <t>TATASTEEL</t>
+  </si>
+  <si>
+    <t>DALBHARAT</t>
+  </si>
+  <si>
+    <t>PFC</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>GLENMARK</t>
+  </si>
+  <si>
+    <t>COALINDIA</t>
+  </si>
+  <si>
+    <t>MUTHOOTFIN</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>DRREDDY</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>IPCALAB</t>
+  </si>
+  <si>
+    <t>SUNPHARMA</t>
+  </si>
+  <si>
+    <t>BALKRISIND</t>
+  </si>
+  <si>
+    <t>ICICIPRULI</t>
+  </si>
+  <si>
+    <t>HCLTECH</t>
+  </si>
+  <si>
+    <t>LTIM</t>
+  </si>
+  <si>
+    <t>DEEPAKNTR</t>
+  </si>
+  <si>
+    <t>CHOLAFIN</t>
+  </si>
+  <si>
+    <t>GAIL</t>
+  </si>
+  <si>
+    <t>VOLTAS</t>
+  </si>
+  <si>
+    <t>ULTRACEMCO</t>
+  </si>
+  <si>
+    <t>CHAMBLFERT</t>
+  </si>
+  <si>
+    <t>APOLLOHOSP</t>
+  </si>
+  <si>
+    <t>INDUSTOWER</t>
+  </si>
+  <si>
+    <t>RBLBANK</t>
+  </si>
+  <si>
+    <t>HINDUNILVR</t>
+  </si>
+  <si>
+    <t>MCX</t>
+  </si>
+  <si>
+    <t>VEDL</t>
+  </si>
+  <si>
+    <t>BHARTIARTL</t>
+  </si>
+  <si>
+    <t>GNFC</t>
+  </si>
+  <si>
+    <t>ITC</t>
+  </si>
+  <si>
+    <t>CROMPTON</t>
+  </si>
+  <si>
+    <t>BANDHANBNK</t>
+  </si>
+  <si>
+    <t>POWERGRID</t>
+  </si>
+  <si>
+    <t>CANFINHOME</t>
+  </si>
+  <si>
+    <t>HAVELLS</t>
+  </si>
+  <si>
+    <t>HINDPETRO</t>
+  </si>
+  <si>
+    <t>M&amp;M</t>
+  </si>
+  <si>
+    <t>ADANIENT</t>
+  </si>
+  <si>
+    <t>POLYCAB</t>
+  </si>
+  <si>
+    <t>SAIL</t>
+  </si>
+  <si>
+    <t>BHARATFORG</t>
+  </si>
+  <si>
+    <t>DIVISLAB</t>
+  </si>
+  <si>
+    <t>IEX</t>
+  </si>
+  <si>
+    <t>MPHASIS</t>
+  </si>
+  <si>
+    <t>SHRIRAMFIN</t>
+  </si>
+  <si>
+    <t>SIEMENS</t>
+  </si>
+  <si>
+    <t>BRITANNIA</t>
+  </si>
+  <si>
+    <t>TATAMOTORS</t>
+  </si>
+  <si>
+    <t>MOTHERSON</t>
+  </si>
+  <si>
+    <t>SBICARD</t>
+  </si>
+  <si>
+    <t>ABCAPITAL</t>
+  </si>
+  <si>
+    <t>BAJFINANCE</t>
+  </si>
+  <si>
+    <t>MRF</t>
+  </si>
+  <si>
+    <t>DIXON</t>
+  </si>
+  <si>
+    <t>IDFCFIRSTB</t>
+  </si>
+  <si>
+    <t>INDIAMART</t>
+  </si>
+  <si>
+    <t>TATACHEM</t>
+  </si>
+  <si>
+    <t>LTF</t>
+  </si>
+  <si>
+    <t>CUB</t>
+  </si>
+  <si>
+    <t>IOC</t>
+  </si>
+  <si>
+    <t>BOSCHLTD</t>
+  </si>
+  <si>
+    <t>ZYDUSLIFE</t>
+  </si>
+  <si>
+    <t>SYNGENE</t>
+  </si>
+  <si>
+    <t>PNB</t>
+  </si>
+  <si>
+    <t>ATUL</t>
+  </si>
+  <si>
+    <t>AUBANK</t>
+  </si>
+  <si>
+    <t>PIIND</t>
+  </si>
+  <si>
+    <t>LALPATHLAB</t>
+  </si>
+  <si>
+    <t>FINNIFTY</t>
+  </si>
+  <si>
+    <t>ABFRL</t>
+  </si>
+  <si>
+    <t>MIDCPNIFTY</t>
+  </si>
+  <si>
+    <t>TATACONSUM</t>
+  </si>
+  <si>
+    <t>IGL</t>
+  </si>
+  <si>
+    <t>NATIONALUM</t>
+  </si>
+  <si>
+    <t>MARUTI</t>
+  </si>
+  <si>
+    <t>SUNTV</t>
+  </si>
+  <si>
+    <t>ALKEM</t>
+  </si>
+  <si>
+    <t>IDFC</t>
+  </si>
+  <si>
+    <t>HDFCLIFE</t>
+  </si>
+  <si>
+    <t>GRANULES</t>
+  </si>
+  <si>
+    <t>NESTLEIND</t>
+  </si>
+  <si>
+    <t>MANAPPURAM</t>
+  </si>
+  <si>
+    <t>ADANIPORTS</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>ASIANPAINT</t>
+  </si>
+  <si>
+    <t>COFORGE</t>
+  </si>
+  <si>
+    <t>ESCORTS</t>
+  </si>
+  <si>
+    <t>BPCL</t>
+  </si>
+  <si>
+    <t>WIPRO</t>
+  </si>
+  <si>
+    <t>NIFTY</t>
+  </si>
+  <si>
+    <t>ASHOKLEY</t>
+  </si>
+  <si>
+    <t>BHEL</t>
+  </si>
+  <si>
+    <t>COLPAL</t>
+  </si>
+  <si>
+    <t>NAVINFLUOR</t>
+  </si>
+  <si>
+    <t>TATAPOWER</t>
+  </si>
+  <si>
+    <t>EXIDEIND</t>
+  </si>
+  <si>
+    <t>BALRAMCHIN</t>
+  </si>
+  <si>
+    <t>CIPLA</t>
+  </si>
+  <si>
+    <t>ASTRAL</t>
+  </si>
+  <si>
+    <t>LUPIN</t>
+  </si>
+  <si>
+    <t>PIDILITIND</t>
+  </si>
+  <si>
+    <t>AXISBANK</t>
+  </si>
+  <si>
+    <t>SRF</t>
+  </si>
+  <si>
+    <t>INDHOTEL</t>
+  </si>
+  <si>
+    <t>ABBOTINDIA</t>
+  </si>
+  <si>
+    <t>TECHM</t>
+  </si>
+  <si>
+    <t>GRASIM</t>
+  </si>
+  <si>
+    <t>ICICIBANK</t>
+  </si>
+  <si>
+    <t>JSWSTEEL</t>
+  </si>
+  <si>
+    <t>AUROPHARMA</t>
+  </si>
+  <si>
+    <t>BATAINDIA</t>
+  </si>
+  <si>
+    <t>INDIGO</t>
+  </si>
+  <si>
+    <t>HDFCBANK</t>
+  </si>
+  <si>
+    <t>APOLLOTYRE</t>
+  </si>
+  <si>
+    <t>TRENT</t>
+  </si>
+  <si>
+    <t>FEDERALBNK</t>
+  </si>
+  <si>
+    <t>GODREJPROP</t>
+  </si>
+  <si>
+    <t>HINDCOPPER</t>
+  </si>
+  <si>
+    <t>TVSMOTOR</t>
+  </si>
+  <si>
+    <t>AMBUJACEM</t>
+  </si>
+  <si>
+    <t>CONCOR</t>
+  </si>
+  <si>
+    <t>BSOFT</t>
+  </si>
+  <si>
+    <t>TORNTPHARM</t>
+  </si>
+  <si>
+    <t>EICHERMOT</t>
+  </si>
+  <si>
+    <t>DABUR</t>
+  </si>
+  <si>
+    <t>HINDALCO</t>
+  </si>
+  <si>
+    <t>MARICO</t>
+  </si>
+  <si>
+    <t>SHREECEM</t>
+  </si>
+  <si>
+    <t>NIFTYNXT50</t>
+  </si>
+  <si>
+    <t>INFY</t>
+  </si>
+  <si>
+    <t>BANKNIFTY</t>
+  </si>
+  <si>
+    <t>IDEA</t>
+  </si>
+  <si>
+    <t>BERGEPAINT</t>
+  </si>
+  <si>
+    <t>DLF</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>IRCTC</t>
+  </si>
+  <si>
+    <t>NTPC</t>
+  </si>
+  <si>
+    <t>LAURUSLABS</t>
+  </si>
+  <si>
+    <t>METROPOLIS</t>
+  </si>
+  <si>
+    <t>CANBK</t>
+  </si>
+  <si>
+    <t>OFSS</t>
+  </si>
+  <si>
+    <t>MGL</t>
+  </si>
+  <si>
+    <t>KOTAKBANK</t>
+  </si>
+  <si>
+    <t>HEROMOTOCO</t>
+  </si>
+  <si>
+    <t>M&amp;MFIN</t>
+  </si>
+  <si>
+    <t>ICICIGI</t>
+  </si>
+  <si>
+    <t>NAUKRI</t>
+  </si>
+  <si>
+    <t>PAGEIND</t>
+  </si>
+  <si>
+    <t>TATACOMM</t>
+  </si>
+  <si>
+    <t>PVRINOX</t>
+  </si>
+  <si>
+    <t>ONGC</t>
+  </si>
+  <si>
+    <t>JUBLFOOD</t>
+  </si>
+  <si>
+    <t>SBIN</t>
+  </si>
+  <si>
+    <t>BIOCON</t>
+  </si>
+  <si>
+    <t>RECLTD</t>
+  </si>
+  <si>
+    <t>JKCEMENT</t>
+  </si>
+  <si>
+    <t>PETRONET</t>
+  </si>
+  <si>
+    <t>UPL</t>
+  </si>
+  <si>
+    <t>GMRINFRA</t>
+  </si>
+  <si>
+    <t>CUMMINSIND</t>
+  </si>
+  <si>
+    <t>BAJAJ-AUTO</t>
+  </si>
+  <si>
+    <t>MFSL</t>
+  </si>
+  <si>
+    <t>INDUSINDBK</t>
+  </si>
+  <si>
+    <t>GODREJCP</t>
+  </si>
+  <si>
+    <t>HDFCAMC</t>
+  </si>
+  <si>
+    <t>UBL</t>
+  </si>
+  <si>
+    <t>PERSISTENT</t>
   </si>
 </sst>
 </file>
@@ -443,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904BEEC-D85C-4382-B015-B596E311D931}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:A186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,60 +976,934 @@
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>